<commit_message>
DCF Update for Cruise Liners
Added other statistical non-GAAP measures: Ticket APCD, Extras PCD, Extras APCD
</commit_message>
<xml_diff>
--- a/DCF Models/CCL.xlsx
+++ b/DCF Models/CCL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\DCF Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF830D82-D271-4E3D-86D0-A02235D0FE2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{167DB3FE-5522-4718-9C75-B3AB51935F4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="3810" windowWidth="32700" windowHeight="15045" activeTab="1" xr2:uid="{3056AFBF-C33C-44A0-B793-E31A92920761}"/>
+    <workbookView xWindow="4020" yWindow="1905" windowWidth="32700" windowHeight="15045" activeTab="1" xr2:uid="{3056AFBF-C33C-44A0-B793-E31A92920761}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="149">
   <si>
     <t>Price</t>
   </si>
@@ -480,22 +480,13 @@
     <t>EBIT</t>
   </si>
   <si>
-    <t>RCL Cash extraction per PCD</t>
-  </si>
-  <si>
-    <t>RCL Cash extraction per APCD</t>
-  </si>
-  <si>
-    <t>RCL Ticket per PCD</t>
-  </si>
-  <si>
-    <t>RCL/NCLH ticket price per APCD</t>
-  </si>
-  <si>
-    <t>RCL/CCL Cash extract per PCD</t>
-  </si>
-  <si>
-    <t>RCL/CCL Cash extract per APCD</t>
+    <t>Extras per PCD</t>
+  </si>
+  <si>
+    <t>Ticket per APCD</t>
+  </si>
+  <si>
+    <t>Extras per APCD</t>
   </si>
 </sst>
 </file>
@@ -682,41 +673,86 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -727,26 +763,8 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -763,59 +781,32 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="3" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1360,26 +1351,26 @@
       </c>
     </row>
     <row r="22" spans="2:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="64" t="s">
+      <c r="B22" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="C22" s="64"/>
-      <c r="D22" s="64"/>
-      <c r="E22" s="65"/>
-      <c r="F22" s="65"/>
-      <c r="G22" s="65"/>
-      <c r="H22" s="66" t="s">
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="I22" s="66"/>
-      <c r="J22" s="66"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="42"/>
     </row>
     <row r="23" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B23" s="67">
+      <c r="B23" s="29">
         <v>2023</v>
       </c>
-      <c r="C23" s="67"/>
-      <c r="D23" s="67"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
       <c r="E23" s="30"/>
       <c r="F23" s="30"/>
       <c r="G23" s="30"/>
@@ -1392,86 +1383,86 @@
       <c r="J23" s="14"/>
     </row>
     <row r="24" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B24" s="60" t="s">
+      <c r="B24" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="60"/>
-      <c r="D24" s="60"/>
-      <c r="E24" s="61"/>
-      <c r="F24" s="61"/>
-      <c r="G24" s="61"/>
-      <c r="H24" s="35" t="s">
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="I24" s="35"/>
+      <c r="I24" s="34"/>
       <c r="J24" s="15"/>
     </row>
     <row r="25" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B25" s="67">
+      <c r="B25" s="29">
         <v>2025</v>
       </c>
-      <c r="C25" s="67"/>
-      <c r="D25" s="67"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
       <c r="E25" s="30"/>
       <c r="F25" s="30"/>
       <c r="G25" s="30"/>
-      <c r="H25" s="47" t="s">
+      <c r="H25" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="I25" s="47"/>
+      <c r="I25" s="31"/>
       <c r="J25" s="16"/>
     </row>
     <row r="26" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B26" s="60">
+      <c r="B26" s="32">
         <v>2026</v>
       </c>
-      <c r="C26" s="60"/>
-      <c r="D26" s="60"/>
-      <c r="E26" s="61"/>
-      <c r="F26" s="61"/>
-      <c r="G26" s="61"/>
-      <c r="H26" s="35" t="s">
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="I26" s="35"/>
+      <c r="I26" s="34"/>
       <c r="J26" s="15"/>
     </row>
     <row r="27" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B27" s="67">
+      <c r="B27" s="29">
         <v>2027</v>
       </c>
-      <c r="C27" s="67"/>
-      <c r="D27" s="67"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
       <c r="E27" s="30"/>
       <c r="F27" s="30"/>
       <c r="G27" s="30"/>
-      <c r="H27" s="47" t="s">
+      <c r="H27" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="I27" s="47"/>
+      <c r="I27" s="31"/>
       <c r="J27" s="16"/>
     </row>
     <row r="28" spans="2:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="60" t="s">
+      <c r="B28" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="C28" s="60"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="61"/>
-      <c r="F28" s="61"/>
-      <c r="G28" s="61"/>
-      <c r="H28" s="50" t="s">
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="33"/>
+      <c r="H28" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="I28" s="50"/>
+      <c r="I28" s="47"/>
       <c r="J28" s="15"/>
     </row>
     <row r="29" spans="2:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="67" t="s">
+      <c r="B29" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="C29" s="67"/>
-      <c r="D29" s="67"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
       <c r="E29" s="30"/>
       <c r="F29" s="30"/>
       <c r="G29" s="30"/>
@@ -1489,221 +1480,221 @@
       </c>
     </row>
     <row r="34" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="68" t="s">
+      <c r="B34" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="C34" s="68"/>
-      <c r="D34" s="68"/>
-      <c r="E34" s="68"/>
-      <c r="F34" s="68"/>
-      <c r="G34" s="68"/>
-      <c r="H34" s="68"/>
-      <c r="I34" s="68"/>
-      <c r="J34" s="68"/>
+      <c r="C34" s="37"/>
+      <c r="D34" s="37"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="37"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="37"/>
+      <c r="I34" s="37"/>
+      <c r="J34" s="37"/>
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B35" s="64" t="s">
+      <c r="B35" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="C35" s="64"/>
-      <c r="D35" s="64"/>
-      <c r="E35" s="65"/>
-      <c r="F35" s="65"/>
-      <c r="G35" s="65"/>
-      <c r="H35" s="70" t="s">
+      <c r="C35" s="38"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="40"/>
+      <c r="F35" s="40"/>
+      <c r="G35" s="40"/>
+      <c r="H35" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="I35" s="70"/>
-      <c r="J35" s="70"/>
-      <c r="K35" s="71"/>
-      <c r="L35" s="71"/>
-      <c r="M35" s="71"/>
-      <c r="N35" s="70" t="s">
+      <c r="I35" s="41"/>
+      <c r="J35" s="41"/>
+      <c r="K35" s="43"/>
+      <c r="L35" s="43"/>
+      <c r="M35" s="43"/>
+      <c r="N35" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="O35" s="70"/>
-      <c r="P35" s="70"/>
+      <c r="O35" s="41"/>
+      <c r="P35" s="41"/>
     </row>
     <row r="36" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="69"/>
-      <c r="C36" s="69"/>
-      <c r="D36" s="69"/>
-      <c r="E36" s="65"/>
-      <c r="F36" s="65"/>
-      <c r="G36" s="65"/>
-      <c r="H36" s="66" t="s">
+      <c r="B36" s="39"/>
+      <c r="C36" s="39"/>
+      <c r="D36" s="39"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="40"/>
+      <c r="G36" s="40"/>
+      <c r="H36" s="42" t="s">
         <v>85</v>
       </c>
-      <c r="I36" s="66"/>
-      <c r="J36" s="66"/>
-      <c r="K36" s="65"/>
-      <c r="L36" s="65"/>
-      <c r="M36" s="65"/>
-      <c r="N36" s="66" t="s">
+      <c r="I36" s="42"/>
+      <c r="J36" s="42"/>
+      <c r="K36" s="40"/>
+      <c r="L36" s="40"/>
+      <c r="M36" s="40"/>
+      <c r="N36" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="O36" s="66"/>
-      <c r="P36" s="66"/>
+      <c r="O36" s="42"/>
+      <c r="P36" s="42"/>
     </row>
     <row r="37" spans="2:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B37" s="72">
+      <c r="B37" s="35">
         <v>2019</v>
       </c>
-      <c r="C37" s="72"/>
-      <c r="D37" s="72"/>
+      <c r="C37" s="35"/>
+      <c r="D37" s="35"/>
       <c r="E37" s="30"/>
       <c r="F37" s="30"/>
       <c r="G37" s="30"/>
-      <c r="H37" s="73" t="s">
+      <c r="H37" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="I37" s="73"/>
+      <c r="I37" s="36"/>
       <c r="J37" s="14"/>
       <c r="K37" s="30"/>
       <c r="L37" s="30"/>
       <c r="M37" s="30"/>
-      <c r="N37" s="73" t="s">
+      <c r="N37" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="O37" s="73"/>
+      <c r="O37" s="36"/>
       <c r="P37" s="14"/>
     </row>
     <row r="38" spans="2:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B38" s="60">
+      <c r="B38" s="32">
         <v>2020</v>
       </c>
-      <c r="C38" s="60"/>
-      <c r="D38" s="60"/>
-      <c r="E38" s="61"/>
-      <c r="F38" s="61"/>
-      <c r="G38" s="61"/>
-      <c r="H38" s="35" t="s">
+      <c r="C38" s="32"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="33"/>
+      <c r="F38" s="33"/>
+      <c r="G38" s="33"/>
+      <c r="H38" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="I38" s="35"/>
+      <c r="I38" s="34"/>
       <c r="J38" s="15"/>
-      <c r="K38" s="61"/>
-      <c r="L38" s="61"/>
-      <c r="M38" s="61"/>
-      <c r="N38" s="35" t="s">
+      <c r="K38" s="33"/>
+      <c r="L38" s="33"/>
+      <c r="M38" s="33"/>
+      <c r="N38" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="O38" s="35"/>
+      <c r="O38" s="34"/>
       <c r="P38" s="15"/>
     </row>
     <row r="39" spans="2:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B39" s="67">
+      <c r="B39" s="29">
         <v>2021</v>
       </c>
-      <c r="C39" s="67"/>
-      <c r="D39" s="67"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="29"/>
       <c r="E39" s="30"/>
       <c r="F39" s="30"/>
       <c r="G39" s="30"/>
-      <c r="H39" s="47" t="s">
+      <c r="H39" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="I39" s="47"/>
+      <c r="I39" s="31"/>
       <c r="J39" s="16"/>
       <c r="K39" s="30"/>
       <c r="L39" s="30"/>
       <c r="M39" s="30"/>
-      <c r="N39" s="47" t="s">
+      <c r="N39" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="O39" s="47"/>
+      <c r="O39" s="31"/>
       <c r="P39" s="16"/>
     </row>
     <row r="40" spans="2:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B40" s="60">
+      <c r="B40" s="32">
         <v>2022</v>
       </c>
-      <c r="C40" s="60"/>
-      <c r="D40" s="60"/>
-      <c r="E40" s="61"/>
-      <c r="F40" s="61"/>
-      <c r="G40" s="61"/>
-      <c r="H40" s="35" t="s">
+      <c r="C40" s="32"/>
+      <c r="D40" s="32"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="33"/>
+      <c r="H40" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="I40" s="35"/>
+      <c r="I40" s="34"/>
       <c r="J40" s="15"/>
-      <c r="K40" s="61"/>
-      <c r="L40" s="61"/>
-      <c r="M40" s="61"/>
-      <c r="N40" s="35" t="s">
+      <c r="K40" s="33"/>
+      <c r="L40" s="33"/>
+      <c r="M40" s="33"/>
+      <c r="N40" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="O40" s="35"/>
+      <c r="O40" s="34"/>
       <c r="P40" s="15"/>
     </row>
     <row r="41" spans="2:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B41" s="67">
+      <c r="B41" s="29">
         <v>2023</v>
       </c>
-      <c r="C41" s="67"/>
-      <c r="D41" s="67"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="29"/>
       <c r="E41" s="30"/>
       <c r="F41" s="30"/>
       <c r="G41" s="30"/>
-      <c r="H41" s="47" t="s">
+      <c r="H41" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="I41" s="47"/>
+      <c r="I41" s="31"/>
       <c r="J41" s="16"/>
       <c r="K41" s="30"/>
       <c r="L41" s="30"/>
       <c r="M41" s="30"/>
-      <c r="N41" s="47" t="s">
+      <c r="N41" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="O41" s="47"/>
+      <c r="O41" s="31"/>
       <c r="P41" s="16"/>
     </row>
     <row r="42" spans="2:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B42" s="60">
+      <c r="B42" s="32">
         <v>2024</v>
       </c>
-      <c r="C42" s="60"/>
-      <c r="D42" s="60"/>
-      <c r="E42" s="61"/>
-      <c r="F42" s="61"/>
-      <c r="G42" s="61"/>
-      <c r="H42" s="35" t="s">
+      <c r="C42" s="32"/>
+      <c r="D42" s="32"/>
+      <c r="E42" s="33"/>
+      <c r="F42" s="33"/>
+      <c r="G42" s="33"/>
+      <c r="H42" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="I42" s="35"/>
+      <c r="I42" s="34"/>
       <c r="J42" s="15"/>
-      <c r="K42" s="61"/>
-      <c r="L42" s="61"/>
-      <c r="M42" s="61"/>
-      <c r="N42" s="35" t="s">
+      <c r="K42" s="33"/>
+      <c r="L42" s="33"/>
+      <c r="M42" s="33"/>
+      <c r="N42" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="O42" s="35"/>
+      <c r="O42" s="34"/>
       <c r="P42" s="15"/>
     </row>
     <row r="43" spans="2:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B43" s="67">
+      <c r="B43" s="29">
         <v>2025</v>
       </c>
-      <c r="C43" s="67"/>
-      <c r="D43" s="67"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="29"/>
       <c r="E43" s="30"/>
       <c r="F43" s="30"/>
       <c r="G43" s="30"/>
-      <c r="H43" s="47" t="s">
+      <c r="H43" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="I43" s="47"/>
+      <c r="I43" s="31"/>
       <c r="J43" s="16"/>
       <c r="K43" s="30"/>
       <c r="L43" s="30"/>
       <c r="M43" s="30"/>
-      <c r="N43" s="47" t="s">
+      <c r="N43" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="O43" s="47"/>
+      <c r="O43" s="31"/>
     </row>
     <row r="47" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B47" s="19" t="s">
@@ -1731,525 +1722,575 @@
       <c r="S48" s="20"/>
     </row>
     <row r="49" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B49" s="58"/>
-      <c r="C49" s="58"/>
-      <c r="D49" s="58"/>
-      <c r="E49" s="62" t="s">
+      <c r="B49" s="44"/>
+      <c r="C49" s="44"/>
+      <c r="D49" s="44"/>
+      <c r="E49" s="45" t="s">
         <v>103</v>
       </c>
-      <c r="F49" s="62"/>
-      <c r="G49" s="62"/>
-      <c r="H49" s="62"/>
-      <c r="I49" s="62"/>
-      <c r="J49" s="62"/>
-      <c r="K49" s="62"/>
-      <c r="L49" s="62"/>
-      <c r="M49" s="62"/>
-      <c r="N49" s="62"/>
-      <c r="O49" s="62"/>
-      <c r="P49" s="62"/>
-      <c r="Q49" s="62"/>
-      <c r="R49" s="62"/>
-      <c r="S49" s="62"/>
+      <c r="F49" s="45"/>
+      <c r="G49" s="45"/>
+      <c r="H49" s="45"/>
+      <c r="I49" s="45"/>
+      <c r="J49" s="45"/>
+      <c r="K49" s="45"/>
+      <c r="L49" s="45"/>
+      <c r="M49" s="45"/>
+      <c r="N49" s="45"/>
+      <c r="O49" s="45"/>
+      <c r="P49" s="45"/>
+      <c r="Q49" s="45"/>
+      <c r="R49" s="45"/>
+      <c r="S49" s="45"/>
     </row>
     <row r="50" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="58"/>
-      <c r="C50" s="58"/>
-      <c r="D50" s="58"/>
-      <c r="E50" s="63" t="s">
+      <c r="B50" s="44"/>
+      <c r="C50" s="44"/>
+      <c r="D50" s="44"/>
+      <c r="E50" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="F50" s="63"/>
-      <c r="G50" s="63"/>
-      <c r="H50" s="63"/>
-      <c r="I50" s="63"/>
-      <c r="J50" s="63"/>
-      <c r="K50" s="63"/>
-      <c r="L50" s="63"/>
-      <c r="M50" s="63"/>
-      <c r="N50" s="63"/>
-      <c r="O50" s="63"/>
-      <c r="P50" s="63"/>
-      <c r="Q50" s="63"/>
-      <c r="R50" s="63"/>
-      <c r="S50" s="63"/>
+      <c r="F50" s="46"/>
+      <c r="G50" s="46"/>
+      <c r="H50" s="46"/>
+      <c r="I50" s="46"/>
+      <c r="J50" s="46"/>
+      <c r="K50" s="46"/>
+      <c r="L50" s="46"/>
+      <c r="M50" s="46"/>
+      <c r="N50" s="46"/>
+      <c r="O50" s="46"/>
+      <c r="P50" s="46"/>
+      <c r="Q50" s="46"/>
+      <c r="R50" s="46"/>
+      <c r="S50" s="46"/>
     </row>
     <row r="51" spans="2:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="58"/>
-      <c r="C51" s="58"/>
-      <c r="D51" s="58"/>
-      <c r="E51" s="56" t="s">
+      <c r="B51" s="44"/>
+      <c r="C51" s="44"/>
+      <c r="D51" s="44"/>
+      <c r="E51" s="48" t="s">
         <v>109</v>
       </c>
-      <c r="F51" s="56"/>
-      <c r="G51" s="56"/>
-      <c r="H51" s="59"/>
-      <c r="I51" s="59"/>
-      <c r="J51" s="59"/>
-      <c r="K51" s="56" t="s">
+      <c r="F51" s="48"/>
+      <c r="G51" s="48"/>
+      <c r="H51" s="52"/>
+      <c r="I51" s="52"/>
+      <c r="J51" s="52"/>
+      <c r="K51" s="48" t="s">
         <v>110</v>
       </c>
-      <c r="L51" s="56"/>
-      <c r="M51" s="56"/>
-      <c r="N51" s="59"/>
-      <c r="O51" s="59"/>
-      <c r="P51" s="59"/>
-      <c r="Q51" s="56" t="s">
+      <c r="L51" s="48"/>
+      <c r="M51" s="48"/>
+      <c r="N51" s="52"/>
+      <c r="O51" s="52"/>
+      <c r="P51" s="52"/>
+      <c r="Q51" s="48" t="s">
         <v>111</v>
       </c>
-      <c r="R51" s="56"/>
-      <c r="S51" s="56"/>
+      <c r="R51" s="48"/>
+      <c r="S51" s="48"/>
     </row>
     <row r="52" spans="2:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="44" t="s">
+      <c r="B52" s="49" t="s">
         <v>105</v>
       </c>
-      <c r="C52" s="44"/>
-      <c r="D52" s="44"/>
-      <c r="E52" s="57"/>
-      <c r="F52" s="57"/>
-      <c r="G52" s="57"/>
-      <c r="H52" s="38"/>
-      <c r="I52" s="38"/>
-      <c r="J52" s="38"/>
-      <c r="K52" s="57"/>
-      <c r="L52" s="57"/>
-      <c r="M52" s="57"/>
-      <c r="N52" s="38"/>
-      <c r="O52" s="38"/>
-      <c r="P52" s="38"/>
-      <c r="Q52" s="57"/>
-      <c r="R52" s="57"/>
-      <c r="S52" s="57"/>
+      <c r="C52" s="49"/>
+      <c r="D52" s="49"/>
+      <c r="E52" s="50"/>
+      <c r="F52" s="50"/>
+      <c r="G52" s="50"/>
+      <c r="H52" s="51"/>
+      <c r="I52" s="51"/>
+      <c r="J52" s="51"/>
+      <c r="K52" s="50"/>
+      <c r="L52" s="50"/>
+      <c r="M52" s="50"/>
+      <c r="N52" s="51"/>
+      <c r="O52" s="51"/>
+      <c r="P52" s="51"/>
+      <c r="Q52" s="50"/>
+      <c r="R52" s="50"/>
+      <c r="S52" s="50"/>
     </row>
     <row r="53" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B53" s="41" t="s">
+      <c r="B53" s="56" t="s">
         <v>112</v>
       </c>
-      <c r="C53" s="41"/>
-      <c r="D53" s="41"/>
-      <c r="E53" s="42">
+      <c r="C53" s="56"/>
+      <c r="D53" s="56"/>
+      <c r="E53" s="57">
         <v>75530</v>
       </c>
-      <c r="F53" s="42"/>
-      <c r="G53" s="42"/>
-      <c r="H53" s="41" t="s">
+      <c r="F53" s="57"/>
+      <c r="G53" s="57"/>
+      <c r="H53" s="56" t="s">
         <v>113</v>
       </c>
-      <c r="I53" s="41"/>
-      <c r="J53" s="41"/>
-      <c r="K53" s="43" t="s">
+      <c r="I53" s="56"/>
+      <c r="J53" s="56"/>
+      <c r="K53" s="58" t="s">
         <v>114</v>
       </c>
-      <c r="L53" s="43"/>
+      <c r="L53" s="58"/>
       <c r="M53" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="N53" s="33"/>
-      <c r="O53" s="33"/>
-      <c r="P53" s="33"/>
-      <c r="Q53" s="35">
+      <c r="N53" s="59"/>
+      <c r="O53" s="59"/>
+      <c r="P53" s="59"/>
+      <c r="Q53" s="34">
         <v>24</v>
       </c>
-      <c r="R53" s="35"/>
-      <c r="S53" s="35"/>
+      <c r="R53" s="34"/>
+      <c r="S53" s="34"/>
     </row>
     <row r="54" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B54" s="36" t="s">
+      <c r="B54" s="53" t="s">
         <v>116</v>
       </c>
-      <c r="C54" s="36"/>
-      <c r="D54" s="36"/>
-      <c r="E54" s="45">
+      <c r="C54" s="53"/>
+      <c r="D54" s="53"/>
+      <c r="E54" s="54">
         <v>46280</v>
       </c>
-      <c r="F54" s="45"/>
-      <c r="G54" s="45"/>
-      <c r="H54" s="38"/>
-      <c r="I54" s="38"/>
-      <c r="J54" s="38"/>
-      <c r="K54" s="46" t="s">
+      <c r="F54" s="54"/>
+      <c r="G54" s="54"/>
+      <c r="H54" s="51"/>
+      <c r="I54" s="51"/>
+      <c r="J54" s="51"/>
+      <c r="K54" s="55" t="s">
         <v>117</v>
       </c>
-      <c r="L54" s="46"/>
+      <c r="L54" s="55"/>
       <c r="M54" s="23"/>
-      <c r="N54" s="38"/>
-      <c r="O54" s="38"/>
-      <c r="P54" s="38"/>
-      <c r="Q54" s="47">
+      <c r="N54" s="51"/>
+      <c r="O54" s="51"/>
+      <c r="P54" s="51"/>
+      <c r="Q54" s="31">
         <v>15</v>
       </c>
-      <c r="R54" s="47"/>
-      <c r="S54" s="47"/>
+      <c r="R54" s="31"/>
+      <c r="S54" s="31"/>
     </row>
     <row r="55" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B55" s="41" t="s">
+      <c r="B55" s="56" t="s">
         <v>118</v>
       </c>
-      <c r="C55" s="41"/>
-      <c r="D55" s="41"/>
-      <c r="E55" s="42">
+      <c r="C55" s="56"/>
+      <c r="D55" s="56"/>
+      <c r="E55" s="57">
         <v>22920</v>
       </c>
-      <c r="F55" s="42"/>
-      <c r="G55" s="42"/>
-      <c r="H55" s="33"/>
-      <c r="I55" s="33"/>
-      <c r="J55" s="33"/>
-      <c r="K55" s="43" t="s">
+      <c r="F55" s="57"/>
+      <c r="G55" s="57"/>
+      <c r="H55" s="59"/>
+      <c r="I55" s="59"/>
+      <c r="J55" s="59"/>
+      <c r="K55" s="58" t="s">
         <v>119</v>
       </c>
-      <c r="L55" s="43"/>
+      <c r="L55" s="58"/>
       <c r="M55" s="21"/>
-      <c r="N55" s="33"/>
-      <c r="O55" s="33"/>
-      <c r="P55" s="33"/>
-      <c r="Q55" s="35">
+      <c r="N55" s="59"/>
+      <c r="O55" s="59"/>
+      <c r="P55" s="59"/>
+      <c r="Q55" s="34">
         <v>11</v>
       </c>
-      <c r="R55" s="35"/>
-      <c r="S55" s="35"/>
+      <c r="R55" s="34"/>
+      <c r="S55" s="34"/>
     </row>
     <row r="56" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B56" s="36" t="s">
+      <c r="B56" s="53" t="s">
         <v>120</v>
       </c>
-      <c r="C56" s="36"/>
-      <c r="D56" s="36"/>
-      <c r="E56" s="45">
+      <c r="C56" s="53"/>
+      <c r="D56" s="53"/>
+      <c r="E56" s="54">
         <v>7230</v>
       </c>
-      <c r="F56" s="45"/>
-      <c r="G56" s="45"/>
-      <c r="H56" s="38"/>
-      <c r="I56" s="38"/>
-      <c r="J56" s="38"/>
-      <c r="K56" s="46" t="s">
+      <c r="F56" s="54"/>
+      <c r="G56" s="54"/>
+      <c r="H56" s="51"/>
+      <c r="I56" s="51"/>
+      <c r="J56" s="51"/>
+      <c r="K56" s="55" t="s">
         <v>121</v>
       </c>
-      <c r="L56" s="46"/>
+      <c r="L56" s="55"/>
       <c r="M56" s="23"/>
-      <c r="N56" s="38"/>
-      <c r="O56" s="38"/>
-      <c r="P56" s="38"/>
-      <c r="Q56" s="47">
+      <c r="N56" s="51"/>
+      <c r="O56" s="51"/>
+      <c r="P56" s="51"/>
+      <c r="Q56" s="31">
         <v>3</v>
       </c>
-      <c r="R56" s="47"/>
-      <c r="S56" s="47"/>
+      <c r="R56" s="31"/>
+      <c r="S56" s="31"/>
     </row>
     <row r="57" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="41" t="s">
+      <c r="B57" s="56" t="s">
         <v>122</v>
       </c>
-      <c r="C57" s="41"/>
-      <c r="D57" s="41"/>
-      <c r="E57" s="54">
+      <c r="C57" s="56"/>
+      <c r="D57" s="56"/>
+      <c r="E57" s="63">
         <v>2840</v>
       </c>
-      <c r="F57" s="54"/>
-      <c r="G57" s="54"/>
-      <c r="H57" s="33"/>
-      <c r="I57" s="33"/>
-      <c r="J57" s="33"/>
-      <c r="K57" s="55" t="s">
+      <c r="F57" s="63"/>
+      <c r="G57" s="63"/>
+      <c r="H57" s="59"/>
+      <c r="I57" s="59"/>
+      <c r="J57" s="59"/>
+      <c r="K57" s="64" t="s">
         <v>123</v>
       </c>
-      <c r="L57" s="55"/>
+      <c r="L57" s="64"/>
       <c r="M57" s="21"/>
-      <c r="N57" s="33"/>
-      <c r="O57" s="33"/>
-      <c r="P57" s="33"/>
-      <c r="Q57" s="50">
+      <c r="N57" s="59"/>
+      <c r="O57" s="59"/>
+      <c r="P57" s="59"/>
+      <c r="Q57" s="47">
         <v>6</v>
       </c>
-      <c r="R57" s="50"/>
-      <c r="S57" s="50"/>
+      <c r="R57" s="47"/>
+      <c r="S57" s="47"/>
     </row>
     <row r="58" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="38"/>
-      <c r="C58" s="38"/>
-      <c r="D58" s="38"/>
-      <c r="E58" s="51">
+      <c r="B58" s="51"/>
+      <c r="C58" s="51"/>
+      <c r="D58" s="51"/>
+      <c r="E58" s="60">
         <v>154800</v>
       </c>
-      <c r="F58" s="51"/>
-      <c r="G58" s="51"/>
-      <c r="H58" s="38"/>
-      <c r="I58" s="38"/>
-      <c r="J58" s="38"/>
-      <c r="K58" s="52" t="s">
+      <c r="F58" s="60"/>
+      <c r="G58" s="60"/>
+      <c r="H58" s="51"/>
+      <c r="I58" s="51"/>
+      <c r="J58" s="51"/>
+      <c r="K58" s="61" t="s">
         <v>124</v>
       </c>
-      <c r="L58" s="52"/>
+      <c r="L58" s="61"/>
       <c r="M58" s="24"/>
-      <c r="N58" s="38"/>
-      <c r="O58" s="38"/>
-      <c r="P58" s="38"/>
-      <c r="Q58" s="53" t="s">
+      <c r="N58" s="51"/>
+      <c r="O58" s="51"/>
+      <c r="P58" s="51"/>
+      <c r="Q58" s="62" t="s">
         <v>125</v>
       </c>
-      <c r="R58" s="53"/>
+      <c r="R58" s="62"/>
       <c r="S58" s="25"/>
     </row>
     <row r="59" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B59" s="33"/>
-      <c r="C59" s="33"/>
-      <c r="D59" s="33"/>
-      <c r="E59" s="49"/>
-      <c r="F59" s="49"/>
-      <c r="G59" s="49"/>
-      <c r="H59" s="33"/>
-      <c r="I59" s="33"/>
-      <c r="J59" s="33"/>
-      <c r="K59" s="49"/>
-      <c r="L59" s="49"/>
-      <c r="M59" s="49"/>
-      <c r="N59" s="33"/>
-      <c r="O59" s="33"/>
-      <c r="P59" s="33"/>
-      <c r="Q59" s="49"/>
-      <c r="R59" s="49"/>
-      <c r="S59" s="49"/>
+      <c r="B59" s="59"/>
+      <c r="C59" s="59"/>
+      <c r="D59" s="59"/>
+      <c r="E59" s="65"/>
+      <c r="F59" s="65"/>
+      <c r="G59" s="65"/>
+      <c r="H59" s="59"/>
+      <c r="I59" s="59"/>
+      <c r="J59" s="59"/>
+      <c r="K59" s="65"/>
+      <c r="L59" s="65"/>
+      <c r="M59" s="65"/>
+      <c r="N59" s="59"/>
+      <c r="O59" s="59"/>
+      <c r="P59" s="59"/>
+      <c r="Q59" s="65"/>
+      <c r="R59" s="65"/>
+      <c r="S59" s="65"/>
     </row>
     <row r="60" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B60" s="36" t="s">
+      <c r="B60" s="53" t="s">
         <v>126</v>
       </c>
-      <c r="C60" s="36"/>
-      <c r="D60" s="36"/>
-      <c r="E60" s="36"/>
-      <c r="F60" s="36"/>
-      <c r="G60" s="36"/>
-      <c r="H60" s="36"/>
-      <c r="I60" s="36"/>
-      <c r="J60" s="36"/>
-      <c r="K60" s="38"/>
-      <c r="L60" s="38"/>
-      <c r="M60" s="38"/>
-      <c r="N60" s="38"/>
-      <c r="O60" s="38"/>
-      <c r="P60" s="38"/>
-      <c r="Q60" s="38"/>
-      <c r="R60" s="38"/>
-      <c r="S60" s="38"/>
+      <c r="C60" s="53"/>
+      <c r="D60" s="53"/>
+      <c r="E60" s="53"/>
+      <c r="F60" s="53"/>
+      <c r="G60" s="53"/>
+      <c r="H60" s="53"/>
+      <c r="I60" s="53"/>
+      <c r="J60" s="53"/>
+      <c r="K60" s="51"/>
+      <c r="L60" s="51"/>
+      <c r="M60" s="51"/>
+      <c r="N60" s="51"/>
+      <c r="O60" s="51"/>
+      <c r="P60" s="51"/>
+      <c r="Q60" s="51"/>
+      <c r="R60" s="51"/>
+      <c r="S60" s="51"/>
     </row>
     <row r="61" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B61" s="48" t="s">
+      <c r="B61" s="66" t="s">
         <v>106</v>
       </c>
-      <c r="C61" s="48"/>
-      <c r="D61" s="48"/>
-      <c r="E61" s="42">
+      <c r="C61" s="66"/>
+      <c r="D61" s="66"/>
+      <c r="E61" s="57">
         <v>39580</v>
       </c>
-      <c r="F61" s="42"/>
-      <c r="G61" s="42"/>
-      <c r="H61" s="41" t="s">
+      <c r="F61" s="57"/>
+      <c r="G61" s="57"/>
+      <c r="H61" s="56" t="s">
         <v>127</v>
       </c>
-      <c r="I61" s="41"/>
-      <c r="J61" s="41"/>
-      <c r="K61" s="43" t="s">
+      <c r="I61" s="56"/>
+      <c r="J61" s="56"/>
+      <c r="K61" s="58" t="s">
         <v>128</v>
       </c>
-      <c r="L61" s="43"/>
+      <c r="L61" s="58"/>
       <c r="M61" s="21"/>
-      <c r="N61" s="33"/>
-      <c r="O61" s="33"/>
-      <c r="P61" s="33"/>
-      <c r="Q61" s="35">
+      <c r="N61" s="59"/>
+      <c r="O61" s="59"/>
+      <c r="P61" s="59"/>
+      <c r="Q61" s="34">
         <v>11</v>
       </c>
-      <c r="R61" s="35"/>
-      <c r="S61" s="35"/>
+      <c r="R61" s="34"/>
+      <c r="S61" s="34"/>
     </row>
     <row r="62" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B62" s="44" t="s">
+      <c r="B62" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C62" s="44"/>
-      <c r="D62" s="44"/>
-      <c r="E62" s="45">
+      <c r="C62" s="49"/>
+      <c r="D62" s="49"/>
+      <c r="E62" s="54">
         <v>33540</v>
       </c>
-      <c r="F62" s="45"/>
-      <c r="G62" s="45"/>
-      <c r="H62" s="36" t="s">
+      <c r="F62" s="54"/>
+      <c r="G62" s="54"/>
+      <c r="H62" s="53" t="s">
         <v>129</v>
       </c>
-      <c r="I62" s="36"/>
-      <c r="J62" s="36"/>
-      <c r="K62" s="46" t="s">
+      <c r="I62" s="53"/>
+      <c r="J62" s="53"/>
+      <c r="K62" s="55" t="s">
         <v>130</v>
       </c>
-      <c r="L62" s="46"/>
+      <c r="L62" s="55"/>
       <c r="M62" s="23"/>
-      <c r="N62" s="38"/>
-      <c r="O62" s="38"/>
-      <c r="P62" s="38"/>
-      <c r="Q62" s="47">
+      <c r="N62" s="51"/>
+      <c r="O62" s="51"/>
+      <c r="P62" s="51"/>
+      <c r="Q62" s="31">
         <v>12</v>
       </c>
-      <c r="R62" s="47"/>
-      <c r="S62" s="47"/>
+      <c r="R62" s="31"/>
+      <c r="S62" s="31"/>
     </row>
     <row r="63" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B63" s="41" t="s">
+      <c r="B63" s="56" t="s">
         <v>131</v>
       </c>
-      <c r="C63" s="41"/>
-      <c r="D63" s="41"/>
-      <c r="E63" s="42">
+      <c r="C63" s="56"/>
+      <c r="D63" s="56"/>
+      <c r="E63" s="57">
         <v>19020</v>
       </c>
-      <c r="F63" s="42"/>
-      <c r="G63" s="42"/>
-      <c r="H63" s="33"/>
-      <c r="I63" s="33"/>
-      <c r="J63" s="33"/>
-      <c r="K63" s="43" t="s">
+      <c r="F63" s="57"/>
+      <c r="G63" s="57"/>
+      <c r="H63" s="59"/>
+      <c r="I63" s="59"/>
+      <c r="J63" s="59"/>
+      <c r="K63" s="58" t="s">
         <v>132</v>
       </c>
-      <c r="L63" s="43"/>
+      <c r="L63" s="58"/>
       <c r="M63" s="21"/>
-      <c r="N63" s="33"/>
-      <c r="O63" s="33"/>
-      <c r="P63" s="33"/>
-      <c r="Q63" s="35">
+      <c r="N63" s="59"/>
+      <c r="O63" s="59"/>
+      <c r="P63" s="59"/>
+      <c r="Q63" s="34">
         <v>6</v>
       </c>
-      <c r="R63" s="35"/>
-      <c r="S63" s="35"/>
+      <c r="R63" s="34"/>
+      <c r="S63" s="34"/>
     </row>
     <row r="64" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="36" t="s">
+      <c r="B64" s="53" t="s">
         <v>133</v>
       </c>
-      <c r="C64" s="36"/>
-      <c r="D64" s="36"/>
-      <c r="E64" s="37">
+      <c r="C64" s="53"/>
+      <c r="D64" s="53"/>
+      <c r="E64" s="67">
         <v>6820</v>
       </c>
-      <c r="F64" s="37"/>
-      <c r="G64" s="37"/>
-      <c r="H64" s="38"/>
-      <c r="I64" s="38"/>
-      <c r="J64" s="38"/>
-      <c r="K64" s="39" t="s">
+      <c r="F64" s="67"/>
+      <c r="G64" s="67"/>
+      <c r="H64" s="51"/>
+      <c r="I64" s="51"/>
+      <c r="J64" s="51"/>
+      <c r="K64" s="68" t="s">
         <v>121</v>
       </c>
-      <c r="L64" s="39"/>
+      <c r="L64" s="68"/>
       <c r="M64" s="23"/>
-      <c r="N64" s="38"/>
-      <c r="O64" s="38"/>
-      <c r="P64" s="38"/>
-      <c r="Q64" s="40">
+      <c r="N64" s="51"/>
+      <c r="O64" s="51"/>
+      <c r="P64" s="51"/>
+      <c r="Q64" s="69">
         <v>3</v>
       </c>
-      <c r="R64" s="40"/>
-      <c r="S64" s="40"/>
+      <c r="R64" s="69"/>
+      <c r="S64" s="69"/>
     </row>
     <row r="65" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="33"/>
-      <c r="C65" s="33"/>
-      <c r="D65" s="33"/>
-      <c r="E65" s="34">
+      <c r="B65" s="59"/>
+      <c r="C65" s="59"/>
+      <c r="D65" s="59"/>
+      <c r="E65" s="73">
         <v>98960</v>
       </c>
-      <c r="F65" s="34"/>
-      <c r="G65" s="34"/>
-      <c r="H65" s="33"/>
-      <c r="I65" s="33"/>
-      <c r="J65" s="33"/>
-      <c r="K65" s="29" t="s">
+      <c r="F65" s="73"/>
+      <c r="G65" s="73"/>
+      <c r="H65" s="59"/>
+      <c r="I65" s="59"/>
+      <c r="J65" s="59"/>
+      <c r="K65" s="70" t="s">
         <v>134</v>
       </c>
-      <c r="L65" s="29"/>
+      <c r="L65" s="70"/>
       <c r="M65" s="26"/>
-      <c r="N65" s="33"/>
-      <c r="O65" s="33"/>
-      <c r="P65" s="33"/>
-      <c r="Q65" s="29" t="s">
+      <c r="N65" s="59"/>
+      <c r="O65" s="59"/>
+      <c r="P65" s="59"/>
+      <c r="Q65" s="70" t="s">
         <v>135</v>
       </c>
-      <c r="R65" s="29"/>
+      <c r="R65" s="70"/>
       <c r="S65" s="26"/>
     </row>
     <row r="66" spans="2:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B66" s="30"/>
       <c r="C66" s="30"/>
       <c r="D66" s="30"/>
-      <c r="E66" s="31">
+      <c r="E66" s="71">
         <v>253760</v>
       </c>
-      <c r="F66" s="31"/>
-      <c r="G66" s="31"/>
+      <c r="F66" s="71"/>
+      <c r="G66" s="71"/>
       <c r="H66" s="30"/>
       <c r="I66" s="30"/>
       <c r="J66" s="30"/>
-      <c r="K66" s="32" t="s">
+      <c r="K66" s="72" t="s">
         <v>136</v>
       </c>
-      <c r="L66" s="32"/>
+      <c r="L66" s="72"/>
       <c r="M66" s="27" t="s">
         <v>115</v>
       </c>
       <c r="N66" s="30"/>
       <c r="O66" s="30"/>
       <c r="P66" s="30"/>
-      <c r="Q66" s="32" t="s">
+      <c r="Q66" s="72" t="s">
         <v>137</v>
       </c>
-      <c r="R66" s="32"/>
+      <c r="R66" s="72"/>
     </row>
     <row r="67" spans="2:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="162">
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="K43:M43"/>
-    <mergeCell ref="N43:O43"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="K42:M42"/>
-    <mergeCell ref="N42:O42"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="K41:M41"/>
-    <mergeCell ref="N41:O41"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="K40:M40"/>
-    <mergeCell ref="N40:O40"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="K37:M37"/>
-    <mergeCell ref="N37:O37"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="K39:M39"/>
-    <mergeCell ref="N39:O39"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="K38:M38"/>
-    <mergeCell ref="N38:O38"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="B34:J34"/>
-    <mergeCell ref="B35:D36"/>
-    <mergeCell ref="E35:G36"/>
-    <mergeCell ref="H35:J35"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="K35:M36"/>
-    <mergeCell ref="N35:P35"/>
-    <mergeCell ref="N36:P36"/>
+    <mergeCell ref="Q65:R65"/>
+    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="E66:G66"/>
+    <mergeCell ref="H66:J66"/>
+    <mergeCell ref="K66:L66"/>
+    <mergeCell ref="N66:P66"/>
+    <mergeCell ref="Q66:R66"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="H65:J65"/>
+    <mergeCell ref="K65:L65"/>
+    <mergeCell ref="N65:P65"/>
+    <mergeCell ref="Q63:S63"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="E64:G64"/>
+    <mergeCell ref="H64:J64"/>
+    <mergeCell ref="K64:L64"/>
+    <mergeCell ref="N64:P64"/>
+    <mergeCell ref="Q64:S64"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="H63:J63"/>
+    <mergeCell ref="K63:L63"/>
+    <mergeCell ref="N63:P63"/>
+    <mergeCell ref="Q61:S61"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="H62:J62"/>
+    <mergeCell ref="K62:L62"/>
+    <mergeCell ref="N62:P62"/>
+    <mergeCell ref="Q62:S62"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="E61:G61"/>
+    <mergeCell ref="H61:J61"/>
+    <mergeCell ref="K61:L61"/>
+    <mergeCell ref="N61:P61"/>
+    <mergeCell ref="Q59:S59"/>
+    <mergeCell ref="B60:J60"/>
+    <mergeCell ref="K60:M60"/>
+    <mergeCell ref="N60:P60"/>
+    <mergeCell ref="Q60:S60"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="E59:G59"/>
+    <mergeCell ref="H59:J59"/>
+    <mergeCell ref="K59:M59"/>
+    <mergeCell ref="N59:P59"/>
+    <mergeCell ref="Q57:S57"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="H58:J58"/>
+    <mergeCell ref="K58:L58"/>
+    <mergeCell ref="N58:P58"/>
+    <mergeCell ref="Q58:R58"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="H57:J57"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="N57:P57"/>
+    <mergeCell ref="Q55:S55"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="H56:J56"/>
+    <mergeCell ref="K56:L56"/>
+    <mergeCell ref="N56:P56"/>
+    <mergeCell ref="Q56:S56"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="H55:J55"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="N55:P55"/>
+    <mergeCell ref="Q53:S53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="H54:J54"/>
+    <mergeCell ref="K54:L54"/>
+    <mergeCell ref="N54:P54"/>
+    <mergeCell ref="Q54:S54"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="H53:J53"/>
+    <mergeCell ref="K53:L53"/>
+    <mergeCell ref="N53:P53"/>
+    <mergeCell ref="Q51:S51"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="H52:J52"/>
+    <mergeCell ref="K52:M52"/>
+    <mergeCell ref="N52:P52"/>
+    <mergeCell ref="Q52:S52"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="H51:J51"/>
+    <mergeCell ref="K51:M51"/>
+    <mergeCell ref="N51:P51"/>
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="E24:G24"/>
     <mergeCell ref="H24:I24"/>
@@ -2274,100 +2315,50 @@
     <mergeCell ref="E28:G28"/>
     <mergeCell ref="H28:I28"/>
     <mergeCell ref="B29:D29"/>
-    <mergeCell ref="Q51:S51"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="H52:J52"/>
-    <mergeCell ref="K52:M52"/>
-    <mergeCell ref="N52:P52"/>
-    <mergeCell ref="Q52:S52"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="H51:J51"/>
-    <mergeCell ref="K51:M51"/>
-    <mergeCell ref="N51:P51"/>
-    <mergeCell ref="Q53:S53"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="H54:J54"/>
-    <mergeCell ref="K54:L54"/>
-    <mergeCell ref="N54:P54"/>
-    <mergeCell ref="Q54:S54"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="H53:J53"/>
-    <mergeCell ref="K53:L53"/>
-    <mergeCell ref="N53:P53"/>
-    <mergeCell ref="Q55:S55"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="H56:J56"/>
-    <mergeCell ref="K56:L56"/>
-    <mergeCell ref="N56:P56"/>
-    <mergeCell ref="Q56:S56"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="H55:J55"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="N55:P55"/>
-    <mergeCell ref="Q57:S57"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="H58:J58"/>
-    <mergeCell ref="K58:L58"/>
-    <mergeCell ref="N58:P58"/>
-    <mergeCell ref="Q58:R58"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="E57:G57"/>
-    <mergeCell ref="H57:J57"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="N57:P57"/>
-    <mergeCell ref="Q59:S59"/>
-    <mergeCell ref="B60:J60"/>
-    <mergeCell ref="K60:M60"/>
-    <mergeCell ref="N60:P60"/>
-    <mergeCell ref="Q60:S60"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="E59:G59"/>
-    <mergeCell ref="H59:J59"/>
-    <mergeCell ref="K59:M59"/>
-    <mergeCell ref="N59:P59"/>
-    <mergeCell ref="Q61:S61"/>
-    <mergeCell ref="B62:D62"/>
-    <mergeCell ref="E62:G62"/>
-    <mergeCell ref="H62:J62"/>
-    <mergeCell ref="K62:L62"/>
-    <mergeCell ref="N62:P62"/>
-    <mergeCell ref="Q62:S62"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="E61:G61"/>
-    <mergeCell ref="H61:J61"/>
-    <mergeCell ref="K61:L61"/>
-    <mergeCell ref="N61:P61"/>
-    <mergeCell ref="Q63:S63"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="E64:G64"/>
-    <mergeCell ref="H64:J64"/>
-    <mergeCell ref="K64:L64"/>
-    <mergeCell ref="N64:P64"/>
-    <mergeCell ref="Q64:S64"/>
-    <mergeCell ref="B63:D63"/>
-    <mergeCell ref="E63:G63"/>
-    <mergeCell ref="H63:J63"/>
-    <mergeCell ref="K63:L63"/>
-    <mergeCell ref="N63:P63"/>
-    <mergeCell ref="Q65:R65"/>
-    <mergeCell ref="B66:D66"/>
-    <mergeCell ref="E66:G66"/>
-    <mergeCell ref="H66:J66"/>
-    <mergeCell ref="K66:L66"/>
-    <mergeCell ref="N66:P66"/>
-    <mergeCell ref="Q66:R66"/>
-    <mergeCell ref="B65:D65"/>
-    <mergeCell ref="E65:G65"/>
-    <mergeCell ref="H65:J65"/>
-    <mergeCell ref="K65:L65"/>
-    <mergeCell ref="N65:P65"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="B34:J34"/>
+    <mergeCell ref="B35:D36"/>
+    <mergeCell ref="E35:G36"/>
+    <mergeCell ref="H35:J35"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="K35:M36"/>
+    <mergeCell ref="N35:P35"/>
+    <mergeCell ref="N36:P36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="K37:M37"/>
+    <mergeCell ref="N37:O37"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="K39:M39"/>
+    <mergeCell ref="N39:O39"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="K38:M38"/>
+    <mergeCell ref="N38:O38"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="K41:M41"/>
+    <mergeCell ref="N41:O41"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="K40:M40"/>
+    <mergeCell ref="N40:O40"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="K43:M43"/>
+    <mergeCell ref="N43:O43"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="K42:M42"/>
+    <mergeCell ref="N42:O42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="597" r:id="rId1"/>
@@ -2379,10 +2370,10 @@
   <dimension ref="A2:DW81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AA63" sqref="AA63"/>
+      <selection pane="bottomRight" activeCell="AB10" sqref="AB10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7952,479 +7943,314 @@
         <v>128.6080586080586</v>
       </c>
     </row>
-    <row r="74" spans="2:27" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="28" t="s">
+    <row r="73" spans="2:27" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="C74" s="28">
-        <v>289.95169082125608</v>
-      </c>
-      <c r="D74" s="28">
-        <v>392.86210462944382</v>
-      </c>
-      <c r="E74" s="28">
-        <v>305.45320855614978</v>
-      </c>
-      <c r="F74" s="28">
-        <v>243.65075034106411</v>
-      </c>
-      <c r="G74" s="28">
-        <v>239.70405297790245</v>
-      </c>
-      <c r="H74" s="28">
-        <v>258.67806767175529</v>
-      </c>
-      <c r="I74" s="28">
-        <v>268.77424568965523</v>
-      </c>
-      <c r="J74" s="28">
-        <v>235.59227573428294</v>
-      </c>
-      <c r="N74" s="28">
-        <v>209.37347679141735</v>
-      </c>
-      <c r="O74" s="28">
-        <v>216.47406679820668</v>
-      </c>
-      <c r="P74" s="28">
-        <v>218.42274233048656</v>
-      </c>
-      <c r="Q74" s="28">
-        <v>223.83350627219733</v>
-      </c>
-      <c r="R74" s="28">
-        <v>219.93590302369924</v>
-      </c>
-      <c r="S74" s="28">
-        <v>215.43156036653426</v>
-      </c>
-      <c r="T74" s="28">
-        <v>211.0911801242236</v>
-      </c>
-      <c r="U74" s="28">
-        <v>219.26585566907298</v>
-      </c>
-      <c r="V74" s="28">
-        <v>226.83750268797934</v>
-      </c>
-      <c r="W74" s="28">
-        <v>244.41274188462788</v>
-      </c>
-      <c r="X74" s="28">
-        <v>253.9471340932798</v>
-      </c>
-      <c r="Y74" s="28">
-        <v>264.04624699831902</v>
-      </c>
-      <c r="Z74" s="28">
-        <v>252.21143504346409</v>
-      </c>
-    </row>
+      <c r="C73" s="28">
+        <f>C4/C65</f>
+        <v>851.85185185185185</v>
+      </c>
+      <c r="D73" s="28">
+        <f t="shared" ref="D73:J73" si="126">D4/D65</f>
+        <v>210.14492753623188</v>
+      </c>
+      <c r="E73" s="28">
+        <f t="shared" si="126"/>
+        <v>118.36337067705797</v>
+      </c>
+      <c r="F73" s="28">
+        <f t="shared" si="126"/>
+        <v>102.16666666666667</v>
+      </c>
+      <c r="G73" s="28">
+        <f t="shared" si="126"/>
+        <v>103.74878959745469</v>
+      </c>
+      <c r="H73" s="28">
+        <f t="shared" si="126"/>
+        <v>97.603638271820898</v>
+      </c>
+      <c r="I73" s="28">
+        <f t="shared" si="126"/>
+        <v>96.666666666666671</v>
+      </c>
+      <c r="J73" s="28">
+        <f t="shared" si="126"/>
+        <v>85.792349726775953</v>
+      </c>
+      <c r="N73" s="28">
+        <f t="shared" ref="N73:Z73" si="127">N4/N65</f>
+        <v>45.198658144100882</v>
+      </c>
+      <c r="O73" s="28">
+        <f t="shared" si="127"/>
+        <v>46.220700980590138</v>
+      </c>
+      <c r="P73" s="28">
+        <f t="shared" si="127"/>
+        <v>46.26344642526972</v>
+      </c>
+      <c r="Q73" s="28">
+        <f t="shared" si="127"/>
+        <v>46.241625757886169</v>
+      </c>
+      <c r="R73" s="28">
+        <f t="shared" si="127"/>
+        <v>50.495474998736036</v>
+      </c>
+      <c r="S73" s="28">
+        <f t="shared" si="127"/>
+        <v>50.766661759099264</v>
+      </c>
+      <c r="T73" s="28">
+        <f t="shared" si="127"/>
+        <v>50.742357503385364</v>
+      </c>
+      <c r="U73" s="28">
+        <f t="shared" si="127"/>
+        <v>52.387090760703586</v>
+      </c>
+      <c r="V73" s="28">
+        <f t="shared" si="127"/>
+        <v>55.220231354366355</v>
+      </c>
+      <c r="W73" s="28">
+        <f t="shared" si="127"/>
+        <v>71.983335938056925</v>
+      </c>
+      <c r="X73" s="28">
+        <f t="shared" si="127"/>
+        <v>72.075471698113205</v>
+      </c>
+      <c r="Y73" s="28">
+        <f t="shared" si="127"/>
+        <v>110.73170731707319</v>
+      </c>
+      <c r="Z73" s="28">
+        <f t="shared" si="127"/>
+        <v>94.26739926739927</v>
+      </c>
+    </row>
+    <row r="74" spans="2:27" s="28" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="75" spans="2:27" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B75" s="28" t="s">
         <v>147</v>
       </c>
       <c r="C75" s="28">
-        <v>109.35450286309215</v>
+        <f>C3/C$66</f>
+        <v>17.341040462427745</v>
       </c>
       <c r="D75" s="28">
-        <v>108.15979600509988</v>
+        <f t="shared" ref="D75:J75" si="128">D3/D$66</f>
+        <v>45.045045045045043</v>
       </c>
       <c r="E75" s="28">
-        <v>111.12791828793775</v>
+        <f t="shared" si="128"/>
+        <v>79.989440337909187</v>
       </c>
       <c r="F75" s="28">
-        <v>144.44493624825617</v>
+        <f t="shared" si="128"/>
+        <v>66.078431372549019</v>
       </c>
       <c r="G75" s="28">
-        <v>137.68903794407831</v>
+        <f t="shared" si="128"/>
+        <v>65.530701095931548</v>
       </c>
       <c r="H75" s="28">
-        <v>212.14269757864781</v>
+        <f t="shared" si="128"/>
+        <v>77.103084123364937</v>
       </c>
       <c r="I75" s="28">
-        <v>258.82653061224494</v>
+        <f t="shared" si="128"/>
+        <v>123.48322626695217</v>
       </c>
       <c r="J75" s="28">
-        <v>223.63215111946101</v>
+        <f t="shared" si="128"/>
+        <v>105.53488372093024</v>
       </c>
       <c r="N75" s="28">
-        <v>218.44937752073935</v>
+        <f t="shared" ref="N75:Z75" si="129">N3/N$66</f>
+        <v>166.56357877868203</v>
       </c>
       <c r="O75" s="28">
-        <v>226.78337921800482</v>
+        <f t="shared" si="129"/>
+        <v>173.75794794693223</v>
       </c>
       <c r="P75" s="28">
-        <v>228.09266116016332</v>
+        <f t="shared" si="129"/>
+        <v>161.97065688562856</v>
       </c>
       <c r="Q75" s="28">
-        <v>234.28835489833639</v>
+        <f t="shared" si="129"/>
+        <v>157.33524239190632</v>
       </c>
       <c r="R75" s="28">
-        <v>232.1811334731795</v>
+        <f t="shared" si="129"/>
+        <v>156.43421052631578</v>
       </c>
       <c r="S75" s="28">
-        <v>226.4619683131105</v>
+        <f t="shared" si="129"/>
+        <v>150.06403042415306</v>
       </c>
       <c r="T75" s="28">
-        <v>224.50785902491248</v>
+        <f t="shared" si="129"/>
+        <v>151.12122196945077</v>
       </c>
       <c r="U75" s="28">
-        <v>237.68336894981192</v>
+        <f t="shared" si="129"/>
+        <v>157.27251740519787</v>
       </c>
       <c r="V75" s="28">
-        <v>247.07234586875359</v>
+        <f t="shared" si="129"/>
+        <v>166.08641739793973</v>
       </c>
       <c r="W75" s="28">
-        <v>264.30145298428033</v>
+        <f t="shared" si="129"/>
+        <v>161.32869692532941</v>
       </c>
       <c r="X75" s="28">
-        <v>258.64520943621955</v>
+        <f t="shared" si="129"/>
+        <v>141.14942528735631</v>
       </c>
       <c r="Y75" s="28">
-        <v>130.20247987646593</v>
+        <f t="shared" si="129"/>
+        <v>68.493150684931507</v>
       </c>
       <c r="Z75" s="28">
-        <v>214.58723980615397</v>
-      </c>
-    </row>
-    <row r="76" spans="2:27" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B76"/>
+        <f t="shared" si="129"/>
+        <v>96.855172413793099</v>
+      </c>
+    </row>
+    <row r="76" spans="2:27" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B76" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="C76" s="28">
+        <f>C4/C$66</f>
+        <v>132.94797687861274</v>
+      </c>
+      <c r="D76" s="28">
+        <f t="shared" ref="C76:J76" si="130">D4/D$66</f>
+        <v>65.315315315315317</v>
+      </c>
+      <c r="E76" s="28">
+        <f t="shared" si="130"/>
+        <v>64.149947201689542</v>
+      </c>
+      <c r="F76" s="28">
+        <f t="shared" si="130"/>
+        <v>60.098039215686278</v>
+      </c>
+      <c r="G76" s="28">
+        <f t="shared" si="130"/>
+        <v>56.297853175198924</v>
+      </c>
+      <c r="H76" s="28">
+        <f t="shared" si="130"/>
+        <v>66.962678507140282</v>
+      </c>
+      <c r="I76" s="28">
+        <f t="shared" si="130"/>
+        <v>81.418034737092555</v>
+      </c>
+      <c r="J76" s="28">
+        <f t="shared" si="130"/>
+        <v>73.023255813953483</v>
+      </c>
+      <c r="N76" s="28">
+        <f t="shared" ref="N76:Z76" si="131">N4/N$66</f>
+        <v>46.645015204712109</v>
+      </c>
+      <c r="O76" s="28">
+        <f t="shared" si="131"/>
+        <v>47.977087617852561</v>
+      </c>
+      <c r="P76" s="28">
+        <f t="shared" si="131"/>
+        <v>48.80793597865955</v>
+      </c>
+      <c r="Q76" s="28">
+        <f t="shared" si="131"/>
+        <v>48.599948671538364</v>
+      </c>
+      <c r="R76" s="28">
+        <f t="shared" si="131"/>
+        <v>52.565789473684212</v>
+      </c>
+      <c r="S76" s="28">
+        <f t="shared" si="131"/>
+        <v>53.203461523536028</v>
+      </c>
+      <c r="T76" s="28">
+        <f t="shared" si="131"/>
+        <v>53.736156596085102</v>
+      </c>
+      <c r="U76" s="28">
+        <f t="shared" si="131"/>
+        <v>55.477929115585098</v>
+      </c>
+      <c r="V76" s="28">
+        <f t="shared" si="131"/>
+        <v>59.030427317817626</v>
+      </c>
+      <c r="W76" s="28">
+        <f t="shared" si="131"/>
+        <v>76.878202781844792</v>
+      </c>
+      <c r="X76" s="28">
+        <f t="shared" si="131"/>
+        <v>73.180076628352481</v>
+      </c>
+      <c r="Y76" s="28">
+        <f t="shared" si="131"/>
+        <v>62.19178082191781</v>
+      </c>
+      <c r="Z76" s="28">
+        <f t="shared" si="131"/>
+        <v>70.993103448275861</v>
+      </c>
     </row>
     <row r="77" spans="2:27" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="28" t="s">
-        <v>150</v>
-      </c>
-      <c r="C77" s="7">
-        <f t="shared" ref="C77:J77" si="126">C74/C69-1</f>
-        <v>-0.69889632107023414</v>
-      </c>
-      <c r="D77" s="7">
-        <f t="shared" si="126"/>
-        <v>0.10642796814006639</v>
-      </c>
-      <c r="E77" s="7">
-        <f t="shared" si="126"/>
-        <v>0.14852644169555962</v>
-      </c>
-      <c r="F77" s="7">
-        <f t="shared" si="126"/>
-        <v>0.13590093399097491</v>
-      </c>
-      <c r="G77" s="7">
-        <f t="shared" si="126"/>
-        <v>6.7665187293442175E-2</v>
-      </c>
-      <c r="H77" s="7">
-        <f t="shared" si="126"/>
-        <v>0.23187214733812977</v>
-      </c>
-      <c r="I77" s="7">
-        <f t="shared" si="126"/>
-        <v>0.10480820917484834</v>
-      </c>
-      <c r="J77" s="7">
-        <f t="shared" si="126"/>
-        <v>0.12303689657134087</v>
-      </c>
-      <c r="N77" s="7">
-        <f>N74/N69-1</f>
-        <v>1.3436766369613107E-2</v>
-      </c>
-      <c r="O77" s="7">
-        <f t="shared" ref="O77:Z77" si="127">O74/O69-1</f>
-        <v>1.3372021991028493E-2</v>
-      </c>
-      <c r="P77" s="7">
-        <f t="shared" si="127"/>
-        <v>9.326089536536486E-2</v>
-      </c>
-      <c r="Q77" s="7">
-        <f t="shared" si="127"/>
-        <v>0.14234489927272165</v>
-      </c>
-      <c r="R77" s="7">
-        <f t="shared" si="127"/>
-        <v>9.5470215539095182E-2</v>
-      </c>
-      <c r="S77" s="7">
-        <f t="shared" si="127"/>
-        <v>0.11071511288303015</v>
-      </c>
-      <c r="T77" s="7">
-        <f t="shared" si="127"/>
-        <v>9.122532620926993E-2</v>
-      </c>
-      <c r="U77" s="7">
-        <f t="shared" si="127"/>
-        <v>9.1431510254739168E-2</v>
-      </c>
-      <c r="V77" s="7">
-        <f t="shared" si="127"/>
-        <v>7.7170794036438117E-2</v>
-      </c>
-      <c r="W77" s="7">
-        <f t="shared" si="127"/>
-        <v>9.5823876863634361E-2</v>
-      </c>
-      <c r="X77" s="7">
-        <f t="shared" si="127"/>
-        <v>0.20300304852912299</v>
-      </c>
-      <c r="Y77" s="7">
-        <f t="shared" si="127"/>
-        <v>0.13478995041206265</v>
-      </c>
-      <c r="Z77" s="7">
-        <f t="shared" si="127"/>
-        <v>0.13162497767878545</v>
-      </c>
+      <c r="B77" s="28"/>
     </row>
     <row r="78" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B78" s="28" t="s">
-        <v>151</v>
-      </c>
-      <c r="C78" s="7">
-        <f t="shared" ref="C78:J78" si="128">C75/C70-1</f>
-        <v>-0.27237196171865619</v>
-      </c>
-      <c r="D78" s="7">
-        <f t="shared" si="128"/>
-        <v>-1.9939807627258221E-2</v>
-      </c>
-      <c r="E78" s="7">
-        <f t="shared" si="128"/>
-        <v>-0.22902462550419755</v>
-      </c>
-      <c r="F78" s="7">
-        <f t="shared" si="128"/>
-        <v>0.14478504252697189</v>
-      </c>
-      <c r="G78" s="7">
-        <f t="shared" si="128"/>
-        <v>0.13018691527480653</v>
-      </c>
-      <c r="H78" s="7">
-        <f>H75/H70-1</f>
-        <v>0.4725406904813596</v>
-      </c>
-      <c r="I78" s="7">
-        <f t="shared" si="128"/>
-        <v>0.26317685573997385</v>
-      </c>
-      <c r="J78" s="7">
-        <f t="shared" si="128"/>
-        <v>0.25243325060391042</v>
-      </c>
-      <c r="N78" s="7">
-        <f>N75/N70-1</f>
-        <v>2.4580545462221881E-2</v>
-      </c>
-      <c r="O78" s="7">
-        <f>O75/O70-1</f>
-        <v>2.2767460452793653E-2</v>
-      </c>
-      <c r="P78" s="7">
-        <f>P75/P70-1</f>
-        <v>8.2143390657432924E-2</v>
-      </c>
-      <c r="Q78" s="7">
-        <f>Q75/Q70-1</f>
-        <v>0.13768003267667184</v>
-      </c>
-      <c r="R78" s="7">
-        <f>R75/R70-1</f>
-        <v>0.11091451422573928</v>
-      </c>
-      <c r="S78" s="7">
-        <f>S75/S70-1</f>
-        <v>0.11410814460873331</v>
-      </c>
-      <c r="T78" s="7">
-        <f>T75/T70-1</f>
-        <v>9.5922737062117625E-2</v>
-      </c>
-      <c r="U78" s="7">
-        <f>U75/U70-1</f>
-        <v>0.11719327896495546</v>
-      </c>
-      <c r="V78" s="7">
-        <f>V75/V70-1</f>
-        <v>9.7529357168799402E-2</v>
-      </c>
-      <c r="W78" s="7">
-        <f>W75/W70-1</f>
-        <v>0.10954574913314397</v>
-      </c>
-      <c r="X78" s="7">
-        <f>X75/X70-1</f>
-        <v>0.20676438439137135</v>
-      </c>
-      <c r="Y78" s="7">
-        <f>Y75/Y70-1</f>
-        <v>-3.6917158299777375E-3</v>
-      </c>
-      <c r="Z78" s="7">
-        <f>Z75/Z70-1</f>
-        <v>0.27845960111316992</v>
-      </c>
+      <c r="B78" s="28"/>
+      <c r="C78" s="7"/>
+      <c r="D78" s="7"/>
+      <c r="E78" s="7"/>
+      <c r="F78" s="7"/>
+      <c r="G78" s="7"/>
+      <c r="H78" s="7"/>
+      <c r="I78" s="7"/>
+      <c r="J78" s="7"/>
+      <c r="N78" s="7"/>
+      <c r="O78" s="7"/>
+      <c r="P78" s="7"/>
+      <c r="Q78" s="7"/>
+      <c r="R78" s="7"/>
+      <c r="S78" s="7"/>
+      <c r="T78" s="7"/>
+      <c r="U78" s="7"/>
+      <c r="V78" s="7"/>
+      <c r="W78" s="7"/>
+      <c r="X78" s="7"/>
+      <c r="Y78" s="7"/>
+      <c r="Z78" s="7"/>
     </row>
     <row r="80" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B80" s="28" t="s">
-        <v>148</v>
-      </c>
-      <c r="C80" s="28">
-        <v>143.85093167701865</v>
-      </c>
-      <c r="D80" s="28">
-        <v>175.9775242740927</v>
-      </c>
-      <c r="E80" s="28">
-        <v>187.26804812834226</v>
-      </c>
-      <c r="F80" s="28">
-        <v>153.14473521021952</v>
-      </c>
-      <c r="G80" s="28">
-        <v>147.51593100453303</v>
-      </c>
-      <c r="H80" s="28">
-        <v>167.9595438018878</v>
-      </c>
-      <c r="I80" s="28">
-        <v>181.48078304597703</v>
-      </c>
-      <c r="J80" s="28">
-        <v>154.02724699989867</v>
-      </c>
-      <c r="N80">
-        <v>152.20129608384238</v>
-      </c>
-      <c r="O80">
-        <v>158.70677201356756</v>
-      </c>
-      <c r="P80">
-        <v>158.94743421463843</v>
-      </c>
-      <c r="Q80">
-        <v>160.92312797194734</v>
-      </c>
-      <c r="R80">
-        <v>160.55153909016616</v>
-      </c>
-      <c r="S80">
-        <v>157.27798977234377</v>
-      </c>
-      <c r="T80">
-        <v>152.77813664596272</v>
-      </c>
-      <c r="U80">
-        <v>157.69914820273274</v>
-      </c>
-      <c r="V80">
-        <v>162.29899887702194</v>
-      </c>
-      <c r="W80">
-        <v>175.36526297132755</v>
-      </c>
-      <c r="X80">
-        <v>172.98085869761789</v>
-      </c>
-      <c r="Y80">
-        <v>162.20365347702111</v>
-      </c>
-      <c r="Z80">
-        <v>165.28305170333135</v>
-      </c>
-    </row>
-    <row r="81" spans="2:26" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="28" t="s">
-        <v>149</v>
-      </c>
-      <c r="C81" s="7">
-        <f t="shared" ref="C81:J81" si="129">C80/C72-1</f>
-        <v>0.29465838509316788</v>
-      </c>
-      <c r="D81" s="7">
-        <f t="shared" si="129"/>
-        <v>0.21424491749123975</v>
-      </c>
-      <c r="E81" s="7">
-        <f t="shared" si="129"/>
-        <v>0.2688491841831242</v>
-      </c>
-      <c r="F81" s="7">
-        <f t="shared" si="129"/>
-        <v>0.36330624816219159</v>
-      </c>
-      <c r="G81" s="7">
-        <f t="shared" si="129"/>
-        <v>0.22152653520248489</v>
-      </c>
-      <c r="H81" s="7">
-        <f t="shared" si="129"/>
-        <v>0.4945131702963308</v>
-      </c>
-      <c r="I81" s="7">
-        <f t="shared" si="129"/>
-        <v>0.23784580343498796</v>
-      </c>
-      <c r="J81" s="7">
-        <f t="shared" si="129"/>
-        <v>0.24226470696260272</v>
-      </c>
-      <c r="N81" s="7">
-        <f>N80/N72-1</f>
-        <v>-5.6986294901653078E-2</v>
-      </c>
-      <c r="O81" s="7">
-        <f t="shared" ref="O81:Z81" si="130">O80/O72-1</f>
-        <v>-5.1913128023381105E-2</v>
-      </c>
-      <c r="P81" s="7">
-        <f t="shared" si="130"/>
-        <v>3.530816211267962E-2</v>
-      </c>
-      <c r="Q81" s="7">
-        <f t="shared" si="130"/>
-        <v>7.4967088919787317E-2</v>
-      </c>
-      <c r="R81" s="7">
-        <f t="shared" si="130"/>
-        <v>6.8398987859162874E-2</v>
-      </c>
-      <c r="S81" s="7">
-        <f t="shared" si="130"/>
-        <v>9.8380023617485435E-2</v>
-      </c>
-      <c r="T81" s="7">
-        <f t="shared" si="130"/>
-        <v>7.0611027356441536E-2</v>
-      </c>
-      <c r="U81" s="7">
-        <f t="shared" si="130"/>
-        <v>6.1872733405960556E-2</v>
-      </c>
-      <c r="V81" s="7">
-        <f t="shared" si="130"/>
-        <v>4.4622627892801026E-2</v>
-      </c>
-      <c r="W81" s="7">
-        <f t="shared" si="130"/>
-        <v>0.16092241754152758</v>
-      </c>
-      <c r="X81" s="7">
-        <f t="shared" si="130"/>
-        <v>0.2442977077868822</v>
-      </c>
-      <c r="Y81" s="7">
-        <f t="shared" si="130"/>
-        <v>0.33006995851157295</v>
-      </c>
-      <c r="Z81" s="7">
-        <f t="shared" si="130"/>
-        <v>0.28516870165222041</v>
-      </c>
+      <c r="B80" s="28"/>
+      <c r="C80" s="28"/>
+      <c r="D80" s="28"/>
+      <c r="E80" s="28"/>
+      <c r="F80" s="28"/>
+      <c r="G80" s="28"/>
+      <c r="H80" s="28"/>
+      <c r="I80" s="28"/>
+      <c r="J80" s="28"/>
+    </row>
+    <row r="81" spans="2:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B81" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>